<commit_message>
Évolution tarification dynamique : m00, m02b-m02d, m03b, interface Streamlit, pipeline évolution
- Config étendue (m00) + config_tarification_dynamique.json, schéma
- m02b types chambre + coefficients par mois
- m02c réservations enrichies (mois, sexe, revenus, pays, province, ville)
- m02d allocation Type_chambre / Numero_chambre
- m03b Rev_Chambre tarification dynamique + Tarif_applique
- Interface Streamlit (interface_streamlit_config.py) + lancer_interface_chrome.sh
- run_pipeline_evolution.py (m02c→m02d→m03b→m04…m09→m10→m11)
- 5 types de chambre par défaut, run_pipeline adapté (14 modules avec règle de blocage)
- Doc : CHAINAGE (pipeline évolution), INTERFACE_UTILISATEUR, ARCHIVE, HISTORIQUE, validated_modules

Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/rapport_validation_sondage_hotel.xlsx
+++ b/rapport_validation_sondage_hotel.xlsx
@@ -513,7 +513,7 @@
         <v>1.4809</v>
       </c>
       <c r="C3" t="n">
-        <v>411.2954</v>
+        <v>516.177</v>
       </c>
       <c r="D3" t="n">
         <v>61.4614</v>
@@ -522,7 +522,7 @@
         <v>51.3048</v>
       </c>
       <c r="F3" t="n">
-        <v>546.7523</v>
+        <v>651.634</v>
       </c>
       <c r="G3" t="n">
         <v>7.5635</v>
@@ -538,7 +538,7 @@
         <v>1.6998</v>
       </c>
       <c r="C4" t="n">
-        <v>502.7635</v>
+        <v>670.7828</v>
       </c>
       <c r="D4" t="n">
         <v>49.6335</v>
@@ -547,7 +547,7 @@
         <v>73.4662</v>
       </c>
       <c r="F4" t="n">
-        <v>545.8373</v>
+        <v>698.2683</v>
       </c>
       <c r="G4" t="n">
         <v>2.1602</v>
@@ -613,7 +613,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>200</v>
+        <v>302.005</v>
       </c>
       <c r="D7" t="n">
         <v>56.4834</v>
@@ -622,7 +622,7 @@
         <v>5.9729</v>
       </c>
       <c r="F7" t="n">
-        <v>374.8753</v>
+        <v>414.8026</v>
       </c>
       <c r="G7" t="n">
         <v>7.5149</v>
@@ -638,7 +638,7 @@
         <v>3</v>
       </c>
       <c r="C8" t="n">
-        <v>700</v>
+        <v>856.75</v>
       </c>
       <c r="D8" t="n">
         <v>86.36790000000001</v>
@@ -647,7 +647,7 @@
         <v>112.0763</v>
       </c>
       <c r="F8" t="n">
-        <v>841.183</v>
+        <v>1014.5591</v>
       </c>
       <c r="G8" t="n">
         <v>8.494</v>
@@ -663,7 +663,7 @@
         <v>9</v>
       </c>
       <c r="C9" t="n">
-        <v>3150</v>
+        <v>6327.23</v>
       </c>
       <c r="D9" t="n">
         <v>214.0162</v>
@@ -672,7 +672,7 @@
         <v>259.8277</v>
       </c>
       <c r="F9" t="n">
-        <v>3487.1382</v>
+        <v>6642.919</v>
       </c>
       <c r="G9" t="n">
         <v>99</v>
@@ -716,7 +716,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2.349171977025976</v>
+        <v>2.349004527793824</v>
       </c>
     </row>
     <row r="3">
@@ -726,7 +726,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.999168542714064</v>
+        <v>0.9994391188903399</v>
       </c>
     </row>
     <row r="4">
@@ -736,7 +736,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.082928697017485</v>
+        <v>1.082739916204542</v>
       </c>
     </row>
     <row r="5">
@@ -746,7 +746,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.295112582232564</v>
+        <v>1.294326892916941</v>
       </c>
     </row>
   </sheetData>
@@ -782,7 +782,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.9996965393722347</v>
+        <v>0.99981413114426</v>
       </c>
       <c r="B2" t="n">
         <v>9499</v>

</xml_diff>

<commit_message>
Saison_calendrier + doc client (Word) + compte rendu
- Ajout module m02e_saison_calendrier (Saison_calendrier dérivée de Mois_sejour)
- Pipeline évolution : m02c → m02e → m02d
- Note Saison vs tarification : .md (doc projet) + .docx (client/prof)
- gen_note_saison_word.py pour régénérer le Word
- run_pipeline.py : 15 modules avec RÈGLE DE BLOCAGE
- validated_modules.txt : m02e ajouté
- COMPTE_RENDU_DERNIERS_CHANGEMENTS.md pour suivi

Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/rapport_validation_sondage_hotel.xlsx
+++ b/rapport_validation_sondage_hotel.xlsx
@@ -513,7 +513,7 @@
         <v>1.4809</v>
       </c>
       <c r="C3" t="n">
-        <v>516.177</v>
+        <v>411.2954</v>
       </c>
       <c r="D3" t="n">
         <v>61.4614</v>
@@ -522,7 +522,7 @@
         <v>51.3048</v>
       </c>
       <c r="F3" t="n">
-        <v>651.634</v>
+        <v>546.7523</v>
       </c>
       <c r="G3" t="n">
         <v>7.5635</v>
@@ -538,7 +538,7 @@
         <v>1.6998</v>
       </c>
       <c r="C4" t="n">
-        <v>670.7828</v>
+        <v>502.7635</v>
       </c>
       <c r="D4" t="n">
         <v>49.6335</v>
@@ -547,7 +547,7 @@
         <v>73.4662</v>
       </c>
       <c r="F4" t="n">
-        <v>698.2683</v>
+        <v>545.8373</v>
       </c>
       <c r="G4" t="n">
         <v>2.1602</v>
@@ -613,7 +613,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>302.005</v>
+        <v>200</v>
       </c>
       <c r="D7" t="n">
         <v>56.4834</v>
@@ -622,7 +622,7 @@
         <v>5.9729</v>
       </c>
       <c r="F7" t="n">
-        <v>414.8026</v>
+        <v>374.8753</v>
       </c>
       <c r="G7" t="n">
         <v>7.5149</v>
@@ -638,7 +638,7 @@
         <v>3</v>
       </c>
       <c r="C8" t="n">
-        <v>856.75</v>
+        <v>700</v>
       </c>
       <c r="D8" t="n">
         <v>86.36790000000001</v>
@@ -647,7 +647,7 @@
         <v>112.0763</v>
       </c>
       <c r="F8" t="n">
-        <v>1014.5591</v>
+        <v>841.183</v>
       </c>
       <c r="G8" t="n">
         <v>8.494</v>
@@ -663,7 +663,7 @@
         <v>9</v>
       </c>
       <c r="C9" t="n">
-        <v>6327.23</v>
+        <v>3150</v>
       </c>
       <c r="D9" t="n">
         <v>214.0162</v>
@@ -672,7 +672,7 @@
         <v>259.8277</v>
       </c>
       <c r="F9" t="n">
-        <v>6642.919</v>
+        <v>3487.1382</v>
       </c>
       <c r="G9" t="n">
         <v>99</v>
@@ -716,7 +716,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2.349004527793824</v>
+        <v>2.349171977025976</v>
       </c>
     </row>
     <row r="3">
@@ -726,7 +726,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9994391188903399</v>
+        <v>0.999168542714064</v>
       </c>
     </row>
     <row r="4">
@@ -736,7 +736,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.082739916204542</v>
+        <v>1.082928697017485</v>
       </c>
     </row>
     <row r="5">
@@ -746,7 +746,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.294326892916941</v>
+        <v>1.295112582232564</v>
       </c>
     </row>
   </sheetData>
@@ -782,7 +782,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.99981413114426</v>
+        <v>0.9996965393722347</v>
       </c>
       <c r="B2" t="n">
         <v>9499</v>

</xml_diff>

<commit_message>
Blocage module, démarche du jour, validation chiffres, régénération CSV + rapport prof
- m11 : RÈGLE DE BLOCAGE confirmée ; section 1 = synthèse validation (chiffres vérifiés sur CSV)
- RAPPORT_DETAILLE : alinéa validation des chiffres (recalcul sur sondage_hotel_data.csv)
- VALIDATION_CHIFFRES_RAPPORT.md : traçabilité rapport ↔ verif_calculs_stats.py
- DEMARCHE_2026-02-24.md : documentation de la démarche (blocage, validation, régénération)
- CSV, Excel, Word prof régénérés (pipeline évolution)

Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/rapport_validation_sondage_hotel.xlsx
+++ b/rapport_validation_sondage_hotel.xlsx
@@ -513,7 +513,7 @@
         <v>1.4809</v>
       </c>
       <c r="C3" t="n">
-        <v>411.2954</v>
+        <v>516.177</v>
       </c>
       <c r="D3" t="n">
         <v>61.4614</v>
@@ -522,7 +522,7 @@
         <v>51.3048</v>
       </c>
       <c r="F3" t="n">
-        <v>546.7523</v>
+        <v>651.634</v>
       </c>
       <c r="G3" t="n">
         <v>7.5635</v>
@@ -538,7 +538,7 @@
         <v>1.6998</v>
       </c>
       <c r="C4" t="n">
-        <v>502.7635</v>
+        <v>670.7828</v>
       </c>
       <c r="D4" t="n">
         <v>49.6335</v>
@@ -547,7 +547,7 @@
         <v>73.4662</v>
       </c>
       <c r="F4" t="n">
-        <v>545.8373</v>
+        <v>698.2683</v>
       </c>
       <c r="G4" t="n">
         <v>2.1602</v>
@@ -613,7 +613,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>200</v>
+        <v>302.005</v>
       </c>
       <c r="D7" t="n">
         <v>56.4834</v>
@@ -622,7 +622,7 @@
         <v>5.9729</v>
       </c>
       <c r="F7" t="n">
-        <v>374.8753</v>
+        <v>414.8026</v>
       </c>
       <c r="G7" t="n">
         <v>7.5149</v>
@@ -638,7 +638,7 @@
         <v>3</v>
       </c>
       <c r="C8" t="n">
-        <v>700</v>
+        <v>856.75</v>
       </c>
       <c r="D8" t="n">
         <v>86.36790000000001</v>
@@ -647,7 +647,7 @@
         <v>112.0763</v>
       </c>
       <c r="F8" t="n">
-        <v>841.183</v>
+        <v>1014.5591</v>
       </c>
       <c r="G8" t="n">
         <v>8.494</v>
@@ -663,7 +663,7 @@
         <v>9</v>
       </c>
       <c r="C9" t="n">
-        <v>3150</v>
+        <v>6327.23</v>
       </c>
       <c r="D9" t="n">
         <v>214.0162</v>
@@ -672,7 +672,7 @@
         <v>259.8277</v>
       </c>
       <c r="F9" t="n">
-        <v>3487.1382</v>
+        <v>6642.919</v>
       </c>
       <c r="G9" t="n">
         <v>99</v>
@@ -716,7 +716,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2.349171977025976</v>
+        <v>2.349004527793824</v>
       </c>
     </row>
     <row r="3">
@@ -726,7 +726,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.999168542714064</v>
+        <v>0.9994391188903399</v>
       </c>
     </row>
     <row r="4">
@@ -736,7 +736,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.082928697017485</v>
+        <v>1.082739916204542</v>
       </c>
     </row>
     <row r="5">
@@ -746,7 +746,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.295112582232564</v>
+        <v>1.294326892916941</v>
       </c>
     </row>
   </sheetData>
@@ -782,7 +782,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.9996965393722347</v>
+        <v>0.99981413114426</v>
       </c>
       <c r="B2" t="n">
         <v>9499</v>

</xml_diff>

<commit_message>
Revenu global (Rev_Banquet), Rev_Spa 80/20 par sexe, Spa×Sexe et tarification dynamique dans m10
- m07: Total_Facture inclut Rev_Banquet (toutes sources)
- m04: ~80% revenus spa depuis F, ~20% M/Autre
- m10: section Lien Spa×Sexe (tableau + ANOVA); section Tarification dynamique (base mensuelle et saison, ANOVA + verdicts); régression avec Rev_Banquet
- Documentation: DEMARCHE_2026-02-24 (trois rapports, modifs récentes, récap Git), RAPPORT_DETAILLE (sections 6, 9, 10, 11)
- Régénération: config.json, sondage_hotel_data.csv, rapport_validation_sondage_hotel.xlsx, synthese_elements_apprentissage_prof.docx

Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/rapport_validation_sondage_hotel.xlsx
+++ b/rapport_validation_sondage_hotel.xlsx
@@ -21,6 +21,12 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Annulations_Canal" sheetId="12" state="visible" r:id="rId12"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Annulations_Resume" sheetId="13" state="visible" r:id="rId13"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Qualite" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Spa_par_sexe" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Spa_sexe_ANOVA" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tarif_dynamique_mensuelle" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tarif_dynamique_mensuelle_ANOVA" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tarif_dynamique_saison" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tarif_dynamique_saison_ANOVA" sheetId="20" state="visible" r:id="rId20"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -438,7 +444,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,20 +465,25 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Rev_Banquet</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Rev_Resto</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Rev_Spa</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Total_Facture</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Satisfaction_NPS</t>
         </is>
@@ -485,22 +496,25 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10522</v>
+        <v>11070</v>
       </c>
       <c r="C2" t="n">
-        <v>10522</v>
+        <v>11070</v>
       </c>
       <c r="D2" t="n">
-        <v>9996</v>
+        <v>11070</v>
       </c>
       <c r="E2" t="n">
-        <v>9996</v>
+        <v>10516</v>
       </c>
       <c r="F2" t="n">
-        <v>10522</v>
+        <v>10516</v>
       </c>
       <c r="G2" t="n">
-        <v>8550</v>
+        <v>11070</v>
+      </c>
+      <c r="H2" t="n">
+        <v>9118</v>
       </c>
     </row>
     <row r="3">
@@ -510,22 +524,25 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.4809</v>
+        <v>1.4931</v>
       </c>
       <c r="C3" t="n">
-        <v>516.177</v>
+        <v>522.3853</v>
       </c>
       <c r="D3" t="n">
-        <v>61.4614</v>
+        <v>66.93259999999999</v>
       </c>
       <c r="E3" t="n">
-        <v>51.3048</v>
+        <v>62.7406</v>
       </c>
       <c r="F3" t="n">
-        <v>651.634</v>
+        <v>34.7169</v>
       </c>
       <c r="G3" t="n">
-        <v>7.5635</v>
+        <v>703.9912</v>
+      </c>
+      <c r="H3" t="n">
+        <v>7.4023</v>
       </c>
     </row>
     <row r="4">
@@ -535,22 +552,25 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.6998</v>
+        <v>1.7018</v>
       </c>
       <c r="C4" t="n">
-        <v>670.7828</v>
+        <v>678.4653</v>
       </c>
       <c r="D4" t="n">
-        <v>49.6335</v>
+        <v>188.7662</v>
       </c>
       <c r="E4" t="n">
-        <v>73.4662</v>
+        <v>49.6676</v>
       </c>
       <c r="F4" t="n">
-        <v>698.2683</v>
+        <v>57.4772</v>
       </c>
       <c r="G4" t="n">
-        <v>2.1602</v>
+        <v>751.8576</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2.0855</v>
       </c>
     </row>
     <row r="5">
@@ -575,7 +595,10 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>4.1976</v>
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>4.2964</v>
       </c>
     </row>
     <row r="6">
@@ -591,16 +614,19 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>21.6524</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
+        <v>23.5177</v>
+      </c>
+      <c r="F6" t="n">
         <v>0</v>
       </c>
-      <c r="F6" t="n">
-        <v>155.6948</v>
-      </c>
       <c r="G6" t="n">
-        <v>6.531</v>
+        <v>146.4553</v>
+      </c>
+      <c r="H6" t="n">
+        <v>6.4182</v>
       </c>
     </row>
     <row r="7">
@@ -616,16 +642,19 @@
         <v>302.005</v>
       </c>
       <c r="D7" t="n">
-        <v>56.4834</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>5.9729</v>
+        <v>58.0985</v>
       </c>
       <c r="F7" t="n">
-        <v>414.8026</v>
+        <v>5.5185</v>
       </c>
       <c r="G7" t="n">
-        <v>7.5149</v>
+        <v>484.8656</v>
+      </c>
+      <c r="H7" t="n">
+        <v>7.282</v>
       </c>
     </row>
     <row r="8">
@@ -638,19 +667,22 @@
         <v>3</v>
       </c>
       <c r="C8" t="n">
-        <v>856.75</v>
+        <v>854.8099999999999</v>
       </c>
       <c r="D8" t="n">
-        <v>86.36790000000001</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>112.0763</v>
+        <v>88.0523</v>
       </c>
       <c r="F8" t="n">
-        <v>1014.5591</v>
+        <v>39.4707</v>
       </c>
       <c r="G8" t="n">
-        <v>8.494</v>
+        <v>1093.2859</v>
+      </c>
+      <c r="H8" t="n">
+        <v>8.065799999999999</v>
       </c>
     </row>
     <row r="9">
@@ -660,21 +692,24 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C9" t="n">
-        <v>6327.23</v>
+        <v>7754.64</v>
       </c>
       <c r="D9" t="n">
-        <v>214.0162</v>
+        <v>2290.0289</v>
       </c>
       <c r="E9" t="n">
-        <v>259.8277</v>
+        <v>206.737</v>
       </c>
       <c r="F9" t="n">
-        <v>6642.919</v>
+        <v>264.3074</v>
       </c>
       <c r="G9" t="n">
+        <v>7860.0154</v>
+      </c>
+      <c r="H9" t="n">
         <v>99</v>
       </c>
     </row>
@@ -689,7 +724,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -716,7 +751,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2.349004527793824</v>
+        <v>2.594250378036349</v>
       </c>
     </row>
     <row r="3">
@@ -726,27 +761,37 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9994391188903399</v>
+        <v>0.9992693475959088</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Rev_Resto</t>
+          <t>Rev_Banquet</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.082739916204542</v>
+        <v>0.9991483920191574</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>Rev_Resto</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1.080593855625323</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>Rev_Spa</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>1.294326892916941</v>
+      <c r="B6" t="n">
+        <v>1.292389857106838</v>
       </c>
     </row>
   </sheetData>
@@ -782,10 +827,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.99981413114426</v>
+        <v>0.9998411752815803</v>
       </c>
       <c r="B2" t="n">
-        <v>9499</v>
+        <v>9984</v>
       </c>
     </row>
   </sheetData>
@@ -836,13 +881,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="C2" t="n">
-        <v>262</v>
+        <v>271</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3779</v>
+        <v>0.2915</v>
       </c>
     </row>
     <row r="3">
@@ -852,13 +897,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="C3" t="n">
-        <v>584</v>
+        <v>555</v>
       </c>
       <c r="D3" t="n">
-        <v>0.286</v>
+        <v>0.2829</v>
       </c>
     </row>
     <row r="4">
@@ -868,13 +913,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>553</v>
+        <v>559</v>
       </c>
       <c r="C4" t="n">
-        <v>1887</v>
+        <v>1921</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2931</v>
+        <v>0.291</v>
       </c>
     </row>
     <row r="5">
@@ -884,13 +929,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C5" t="n">
-        <v>1585</v>
+        <v>1640</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0732</v>
+        <v>0.06710000000000001</v>
       </c>
     </row>
     <row r="6">
@@ -900,13 +945,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="C6" t="n">
-        <v>981</v>
+        <v>1106</v>
       </c>
       <c r="D6" t="n">
-        <v>0.3303</v>
+        <v>0.2821</v>
       </c>
     </row>
     <row r="7">
@@ -916,13 +961,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="C7" t="n">
-        <v>237</v>
+        <v>284</v>
       </c>
       <c r="D7" t="n">
-        <v>0.3502</v>
+        <v>0.3204</v>
       </c>
     </row>
     <row r="8">
@@ -932,13 +977,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C8" t="n">
-        <v>417</v>
+        <v>431</v>
       </c>
       <c r="D8" t="n">
-        <v>0.3046</v>
+        <v>0.2715</v>
       </c>
     </row>
     <row r="9">
@@ -948,13 +993,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="C9" t="n">
-        <v>2120</v>
+        <v>2246</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0618</v>
+        <v>0.0663</v>
       </c>
     </row>
     <row r="10">
@@ -964,13 +1009,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="C10" t="n">
-        <v>342</v>
+        <v>314</v>
       </c>
       <c r="D10" t="n">
-        <v>0.2924</v>
+        <v>0.2834</v>
       </c>
     </row>
     <row r="11">
@@ -980,13 +1025,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C11" t="n">
-        <v>276</v>
+        <v>293</v>
       </c>
       <c r="D11" t="n">
-        <v>0.2935</v>
+        <v>0.2628</v>
       </c>
     </row>
     <row r="12">
@@ -996,13 +1041,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="C12" t="n">
-        <v>313</v>
+        <v>334</v>
       </c>
       <c r="D12" t="n">
-        <v>0.262</v>
+        <v>0.2934</v>
       </c>
     </row>
     <row r="13">
@@ -1012,13 +1057,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C13" t="n">
-        <v>1518</v>
+        <v>1675</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0718</v>
+        <v>0.06809999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1054,10 +1099,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.0681600612674708</v>
+        <v>0.06707426721812623</v>
       </c>
       <c r="B2" t="n">
-        <v>0.3049632006038875</v>
+        <v>0.286621891450354</v>
       </c>
     </row>
   </sheetData>
@@ -1118,7 +1163,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>526</v>
+        <v>554</v>
       </c>
     </row>
     <row r="5">
@@ -1128,7 +1173,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>526</v>
+        <v>554</v>
       </c>
     </row>
     <row r="6">
@@ -1139,6 +1184,444 @@
       </c>
       <c r="B6" t="n">
         <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Sexe</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Effectif</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Moyenne_Rev_Spa</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Somme_Rev_Spa</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Pct_du_total_Rev_Spa</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Pct_avec_Rev_Spa_gt_0</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Autre</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>224</v>
+      </c>
+      <c r="C2" t="n">
+        <v>15.61</v>
+      </c>
+      <c r="D2" t="n">
+        <v>3496.62</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>45.9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>5212</v>
+      </c>
+      <c r="C3" t="n">
+        <v>52.49</v>
+      </c>
+      <c r="D3" t="n">
+        <v>273591.21</v>
+      </c>
+      <c r="E3" t="n">
+        <v>74.90000000000001</v>
+      </c>
+      <c r="F3" t="n">
+        <v>53.6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>5080</v>
+      </c>
+      <c r="C4" t="n">
+        <v>17.32</v>
+      </c>
+      <c r="D4" t="n">
+        <v>87995.59</v>
+      </c>
+      <c r="E4" t="n">
+        <v>24.1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>50.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>F_ANOVA</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>p_value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>545.4545715651002</v>
+      </c>
+      <c r="B2" t="n">
+        <v>4.107760137958238e-226</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Mois_sejour</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Effectif</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Moyenne_Tarif_applique</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>431</v>
+      </c>
+      <c r="C2" t="n">
+        <v>255.18</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>451</v>
+      </c>
+      <c r="C3" t="n">
+        <v>286.78</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>507</v>
+      </c>
+      <c r="C4" t="n">
+        <v>346.81</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>496</v>
+      </c>
+      <c r="C5" t="n">
+        <v>356.56</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>554</v>
+      </c>
+      <c r="C6" t="n">
+        <v>364.28</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>596</v>
+      </c>
+      <c r="C7" t="n">
+        <v>414.13</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>608</v>
+      </c>
+      <c r="C8" t="n">
+        <v>383.88</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>629</v>
+      </c>
+      <c r="C9" t="n">
+        <v>426.18</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>558</v>
+      </c>
+      <c r="C10" t="n">
+        <v>378.42</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>560</v>
+      </c>
+      <c r="C11" t="n">
+        <v>352.49</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n">
+        <v>525</v>
+      </c>
+      <c r="C12" t="n">
+        <v>324.18</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="n">
+        <v>449</v>
+      </c>
+      <c r="C13" t="n">
+        <v>241.47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>F_ANOVA</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>p_value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>93.71625569619539</v>
+      </c>
+      <c r="B2" t="n">
+        <v>5.705318355837312e-198</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Saison_calendrier</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Effectif</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Moyenne_Tarif_applique</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Basse</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1331</v>
+      </c>
+      <c r="C2" t="n">
+        <v>261.26</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Haute</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1833</v>
+      </c>
+      <c r="C3" t="n">
+        <v>408.23</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Épaule</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>3200</v>
+      </c>
+      <c r="C4" t="n">
+        <v>354.14</v>
       </c>
     </row>
   </sheetData>
@@ -1179,7 +1662,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2631</v>
+        <v>2766</v>
       </c>
     </row>
     <row r="3">
@@ -1189,7 +1672,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2105</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="4">
@@ -1199,7 +1682,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2103</v>
+        <v>2214</v>
       </c>
     </row>
     <row r="5">
@@ -1209,7 +1692,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1053</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="6">
@@ -1219,7 +1702,46 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2630</v>
+        <v>2767</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>F_ANOVA</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>p_value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>454.4217295766898</v>
+      </c>
+      <c r="B2" t="n">
+        <v>3.404625962493534e-185</v>
       </c>
     </row>
   </sheetData>
@@ -1260,7 +1782,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8550</v>
+        <v>9118</v>
       </c>
     </row>
     <row r="3">
@@ -1270,7 +1792,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1972</v>
+        <v>1952</v>
       </c>
     </row>
   </sheetData>
@@ -1321,13 +1843,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.187416840904771</v>
+        <v>0.1763324299909666</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1799601672250971</v>
+        <v>0.1692329859453738</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1948735145844449</v>
+        <v>0.1834318740365593</v>
       </c>
     </row>
     <row r="3">
@@ -1337,13 +1859,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.5234746245960844</v>
+        <v>0.520776874435411</v>
       </c>
       <c r="C3" t="n">
-        <v>0.5139313426283647</v>
+        <v>0.5114705756882526</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5330179065638041</v>
+        <v>0.5300831731825694</v>
       </c>
     </row>
     <row r="4">
@@ -1353,13 +1875,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.420547424444022</v>
+        <v>0.4164408310749774</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4111149994546705</v>
+        <v>0.4072574763157693</v>
       </c>
       <c r="D4" t="n">
-        <v>0.4299798494333736</v>
+        <v>0.4256241858341856</v>
       </c>
     </row>
   </sheetData>
@@ -1405,10 +1927,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1775</v>
+        <v>1934</v>
       </c>
       <c r="C2" t="n">
-        <v>856</v>
+        <v>832</v>
       </c>
     </row>
     <row r="3">
@@ -1418,10 +1940,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1897</v>
+        <v>1994</v>
       </c>
       <c r="C3" t="n">
-        <v>208</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4">
@@ -1431,10 +1953,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1015</v>
+        <v>1093</v>
       </c>
       <c r="C4" t="n">
-        <v>1088</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="5">
@@ -1444,10 +1966,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>869</v>
+        <v>911</v>
       </c>
       <c r="C5" t="n">
-        <v>184</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6">
@@ -1457,10 +1979,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>541</v>
+        <v>528</v>
       </c>
       <c r="C6" t="n">
-        <v>2089</v>
+        <v>2239</v>
       </c>
     </row>
   </sheetData>
@@ -1501,7 +2023,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2841.562106440745</v>
+        <v>3155.683610447935</v>
       </c>
       <c r="B2" t="n">
         <v>4</v>
@@ -1548,13 +2070,13 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.4475709066127099</v>
+        <v>0.4556048877432787</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>8121</v>
+        <v>8657</v>
       </c>
     </row>
   </sheetData>
@@ -1600,10 +2122,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>60.204</v>
+        <v>60.7612</v>
       </c>
       <c r="C2" t="n">
-        <v>2041</v>
+        <v>2125</v>
       </c>
     </row>
     <row r="3">
@@ -1613,10 +2135,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>45.0409</v>
+        <v>45.3353</v>
       </c>
       <c r="C3" t="n">
-        <v>1625</v>
+        <v>1742</v>
       </c>
     </row>
     <row r="4">
@@ -1626,10 +2148,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>149.7413</v>
+        <v>149.6171</v>
       </c>
       <c r="C4" t="n">
-        <v>1605</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="5">
@@ -1639,10 +2161,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>21.4728</v>
+        <v>20.7329</v>
       </c>
       <c r="C5" t="n">
-        <v>820</v>
+        <v>876</v>
       </c>
     </row>
     <row r="6">
@@ -1652,10 +2174,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>79.3849</v>
+        <v>79.95869999999999</v>
       </c>
       <c r="C6" t="n">
-        <v>2020</v>
+        <v>2181</v>
       </c>
     </row>
   </sheetData>
@@ -1691,7 +2213,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>10362.83764784444</v>
+        <v>10924.19889194672</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>

</xml_diff>